<commit_message>
Updated GSX results spreadsheet
</commit_message>
<xml_diff>
--- a/GSX Results.xlsx
+++ b/GSX Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swiftteamsix/Dropbox/Business/Yolo Capital/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A097F73-B09B-794D-AF2B-32C30CB4E0AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6092E75-7E60-AD4C-8C8A-07CCE0457B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38760" yWindow="460" windowWidth="38040" windowHeight="42740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="76080" windowHeight="42740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -136,18 +136,18 @@
     <t>$27.0M</t>
   </si>
   <si>
+    <t>09:48:37</t>
+  </si>
+  <si>
+    <t>$5.0M</t>
+  </si>
+  <si>
     <t>15:50:06</t>
   </si>
   <si>
     <t>$18.0M</t>
   </si>
   <si>
-    <t>09:48:37</t>
-  </si>
-  <si>
-    <t>$5.0M</t>
-  </si>
-  <si>
     <t>11:58:20</t>
   </si>
   <si>
@@ -193,35 +193,178 @@
     <t>$20.0M</t>
   </si>
   <si>
+    <t>13:46:58</t>
+  </si>
+  <si>
+    <t>$8.7M</t>
+  </si>
+  <si>
+    <t>14:18:41</t>
+  </si>
+  <si>
+    <t>$7.0M</t>
+  </si>
+  <si>
     <t>15:02:39</t>
   </si>
   <si>
-    <t>$8.7M</t>
-  </si>
-  <si>
-    <t>13:46:58</t>
-  </si>
-  <si>
-    <t>14:18:41</t>
-  </si>
-  <si>
-    <t>$7.0M</t>
-  </si>
-  <si>
     <t>13:53:50</t>
   </si>
   <si>
     <t>$5.3M</t>
+  </si>
+  <si>
+    <t>15:49:52</t>
+  </si>
+  <si>
+    <t>$28.0M</t>
+  </si>
+  <si>
+    <t>13:10:29</t>
+  </si>
+  <si>
+    <t>$7.6M</t>
+  </si>
+  <si>
+    <t>16:36:41</t>
+  </si>
+  <si>
+    <t>$30.0M</t>
+  </si>
+  <si>
+    <t>16:22:35</t>
+  </si>
+  <si>
+    <t>16:34:21</t>
+  </si>
+  <si>
+    <t>$10.0M</t>
+  </si>
+  <si>
+    <t>16:30:44</t>
+  </si>
+  <si>
+    <t>$5.2M</t>
+  </si>
+  <si>
+    <t>15:01:40</t>
+  </si>
+  <si>
+    <t>$6.1M</t>
+  </si>
+  <si>
+    <t>14:52:56</t>
+  </si>
+  <si>
+    <t>$7.8M</t>
+  </si>
+  <si>
+    <t>15:34:46</t>
+  </si>
+  <si>
+    <t>14:53:13</t>
+  </si>
+  <si>
+    <t>$6.9M</t>
+  </si>
+  <si>
+    <t>16:27:41</t>
+  </si>
+  <si>
+    <t>15:25:31</t>
+  </si>
+  <si>
+    <t>15:53:51</t>
+  </si>
+  <si>
+    <t>$19.0M</t>
+  </si>
+  <si>
+    <t>15:36:20</t>
+  </si>
+  <si>
+    <t>15:34:54</t>
+  </si>
+  <si>
+    <t>$85.0M</t>
+  </si>
+  <si>
+    <t>13:59:12</t>
+  </si>
+  <si>
+    <t>12:19:05</t>
+  </si>
+  <si>
+    <t>$6.4M</t>
+  </si>
+  <si>
+    <t>10:46:26</t>
+  </si>
+  <si>
+    <t>$8.1M</t>
+  </si>
+  <si>
+    <t>16:33:25</t>
+  </si>
+  <si>
+    <t>$52.0M</t>
+  </si>
+  <si>
+    <t>12:53:58</t>
+  </si>
+  <si>
+    <t>15:49:21</t>
+  </si>
+  <si>
+    <t>15:08:12</t>
+  </si>
+  <si>
+    <t>$180.0M</t>
+  </si>
+  <si>
+    <t>14:57:25</t>
+  </si>
+  <si>
+    <t>12:31:10</t>
+  </si>
+  <si>
+    <t>$9.8M</t>
+  </si>
+  <si>
+    <t>12:42:40</t>
+  </si>
+  <si>
+    <t>$7.5M</t>
+  </si>
+  <si>
+    <t>16:06:44</t>
+  </si>
+  <si>
+    <t>$87.0M</t>
+  </si>
+  <si>
+    <t>16:22:00</t>
+  </si>
+  <si>
+    <t>$66.0M</t>
+  </si>
+  <si>
+    <t>15:01:25</t>
+  </si>
+  <si>
+    <t>$60.0M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +376,19 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -267,20 +423,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -578,18 +761,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -603,7 +789,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -629,7 +815,7 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>1000000</v>
       </c>
       <c r="E2">
@@ -655,7 +841,7 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>1000000</v>
       </c>
       <c r="E3">
@@ -681,7 +867,7 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>750000</v>
       </c>
       <c r="E4">
@@ -707,7 +893,7 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>174900</v>
       </c>
       <c r="E5">
@@ -733,7 +919,7 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>967840</v>
       </c>
       <c r="E6">
@@ -759,7 +945,7 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>500000</v>
       </c>
       <c r="E7">
@@ -785,7 +971,7 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>250000</v>
       </c>
       <c r="E8">
@@ -811,7 +997,7 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>275000</v>
       </c>
       <c r="E9">
@@ -837,7 +1023,7 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>830000</v>
       </c>
       <c r="E10">
@@ -863,7 +1049,7 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>500000</v>
       </c>
       <c r="E11">
@@ -889,7 +1075,7 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>400000</v>
       </c>
       <c r="E12">
@@ -915,7 +1101,7 @@
       <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>750000</v>
       </c>
       <c r="E13">
@@ -941,7 +1127,7 @@
       <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>200000</v>
       </c>
       <c r="E14">
@@ -967,7 +1153,7 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>800000</v>
       </c>
       <c r="E15">
@@ -993,14 +1179,14 @@
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D16">
-        <v>550000</v>
+      <c r="D16" s="4">
+        <v>158500</v>
       </c>
       <c r="E16">
-        <v>32.78</v>
+        <v>32</v>
       </c>
       <c r="F16">
-        <v>0.1235</v>
+        <v>3.56E-2</v>
       </c>
       <c r="G16" t="s">
         <v>39</v>
@@ -1019,14 +1205,14 @@
       <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D17">
-        <v>158500</v>
+      <c r="D17" s="4">
+        <v>550000</v>
       </c>
       <c r="E17">
-        <v>32</v>
+        <v>32.78</v>
       </c>
       <c r="F17">
-        <v>3.56E-2</v>
+        <v>0.1235</v>
       </c>
       <c r="G17" t="s">
         <v>41</v>
@@ -1045,7 +1231,7 @@
       <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>200000</v>
       </c>
       <c r="E18">
@@ -1071,7 +1257,7 @@
       <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>1325000</v>
       </c>
       <c r="E19">
@@ -1097,7 +1283,7 @@
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>150000</v>
       </c>
       <c r="E20">
@@ -1123,7 +1309,7 @@
       <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>160000</v>
       </c>
       <c r="E21">
@@ -1149,7 +1335,7 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>300000</v>
       </c>
       <c r="E22">
@@ -1175,7 +1361,7 @@
       <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>125000</v>
       </c>
       <c r="E23">
@@ -1201,7 +1387,7 @@
       <c r="C24" t="s">
         <v>9</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>520515</v>
       </c>
       <c r="E24">
@@ -1227,7 +1413,7 @@
       <c r="C25" t="s">
         <v>9</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>500000</v>
       </c>
       <c r="E25">
@@ -1253,11 +1439,11 @@
       <c r="C26" t="s">
         <v>9</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <v>250000</v>
       </c>
       <c r="E26">
-        <v>34.93</v>
+        <v>35.15</v>
       </c>
       <c r="F26">
         <v>4.6399999999999997E-2</v>
@@ -1266,7 +1452,7 @@
         <v>58</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1279,17 +1465,17 @@
       <c r="C27" t="s">
         <v>9</v>
       </c>
-      <c r="D27">
-        <v>250000</v>
+      <c r="D27" s="4">
+        <v>200000</v>
       </c>
       <c r="E27">
-        <v>35.15</v>
+        <v>35.229999999999997</v>
       </c>
       <c r="F27">
-        <v>4.6399999999999997E-2</v>
+        <v>3.7100000000000001E-2</v>
       </c>
       <c r="G27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H27" t="s">
         <v>14</v>
@@ -1300,25 +1486,25 @@
         <v>43965</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="D28">
-        <v>200000</v>
+      <c r="D28" s="4">
+        <v>250000</v>
       </c>
       <c r="E28">
-        <v>35.229999999999997</v>
+        <v>34.93</v>
       </c>
       <c r="F28">
-        <v>3.7100000000000001E-2</v>
+        <v>4.6399999999999997E-2</v>
       </c>
       <c r="G28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1331,7 +1517,7 @@
       <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>150000</v>
       </c>
       <c r="E29">
@@ -1347,7 +1533,740 @@
         <v>14</v>
       </c>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>43970</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="4">
+        <v>839214</v>
+      </c>
+      <c r="E30">
+        <v>33.880000000000003</v>
+      </c>
+      <c r="F30">
+        <v>0.153</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>43971</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="4">
+        <v>250000</v>
+      </c>
+      <c r="E31">
+        <v>30.5</v>
+      </c>
+      <c r="F31">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>43971</v>
+      </c>
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="E32">
+        <v>30.58</v>
+      </c>
+      <c r="F32">
+        <v>0.1648</v>
+      </c>
+      <c r="G32" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>43973</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="4">
+        <v>433037</v>
+      </c>
+      <c r="E33">
+        <v>29.73</v>
+      </c>
+      <c r="F33">
+        <v>6.88E-2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="4">
+        <v>353210</v>
+      </c>
+      <c r="E34">
+        <v>29.77</v>
+      </c>
+      <c r="F34">
+        <v>5.4399999999999997E-2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="4">
+        <v>174831</v>
+      </c>
+      <c r="E35">
+        <v>29.85</v>
+      </c>
+      <c r="F35">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>74</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="4">
+        <v>195099</v>
+      </c>
+      <c r="E36">
+        <v>31.359200000000001</v>
+      </c>
+      <c r="F36">
+        <v>3.27E-2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="4">
+        <v>250000</v>
+      </c>
+      <c r="E37">
+        <v>31.46</v>
+      </c>
+      <c r="F37">
+        <v>4.19E-2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1150000</v>
+      </c>
+      <c r="E38">
+        <v>32.61</v>
+      </c>
+      <c r="F38">
+        <v>0.19270000000000001</v>
+      </c>
+      <c r="G38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="4">
+        <v>175000</v>
+      </c>
+      <c r="E39">
+        <v>39.450000000000003</v>
+      </c>
+      <c r="F39">
+        <v>2.7E-2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="4">
+        <v>500000</v>
+      </c>
+      <c r="E40">
+        <v>41.4</v>
+      </c>
+      <c r="F40">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E41">
+        <v>40.520000000000003</v>
+      </c>
+      <c r="F41">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>32</v>
+      </c>
+      <c r="H41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="4">
+        <v>495589</v>
+      </c>
+      <c r="E42">
+        <v>39.6</v>
+      </c>
+      <c r="F42">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="4">
+        <v>576867</v>
+      </c>
+      <c r="E43">
+        <v>40.97</v>
+      </c>
+      <c r="F43">
+        <v>8.6599999999999996E-2</v>
+      </c>
+      <c r="G43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="4">
+        <v>2154123</v>
+      </c>
+      <c r="E44">
+        <v>39.5</v>
+      </c>
+      <c r="F44">
+        <v>0.32479999999999998</v>
+      </c>
+      <c r="G44" t="s">
+        <v>88</v>
+      </c>
+      <c r="H44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="4">
+        <v>400000</v>
+      </c>
+      <c r="E45">
+        <v>41.6</v>
+      </c>
+      <c r="F45">
+        <v>5.9900000000000002E-2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="4">
+        <v>125000</v>
+      </c>
+      <c r="E46">
+        <v>51.7</v>
+      </c>
+      <c r="F46">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="G46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="4">
+        <v>150000</v>
+      </c>
+      <c r="E47">
+        <v>54.5</v>
+      </c>
+      <c r="F47">
+        <v>2.24E-2</v>
+      </c>
+      <c r="G47" t="s">
+        <v>93</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="E48">
+        <v>52</v>
+      </c>
+      <c r="F48">
+        <v>0.14929999999999999</v>
+      </c>
+      <c r="G48" t="s">
+        <v>95</v>
+      </c>
+      <c r="H48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="4">
+        <v>100000</v>
+      </c>
+      <c r="E49">
+        <v>52.15</v>
+      </c>
+      <c r="F49">
+        <v>1.49E-2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>74</v>
+      </c>
+      <c r="H49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="4">
+        <v>500000</v>
+      </c>
+      <c r="E50">
+        <v>51.78</v>
+      </c>
+      <c r="F50">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>28</v>
+      </c>
+      <c r="H50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="4">
+        <v>3215364</v>
+      </c>
+      <c r="E51">
+        <v>56.16</v>
+      </c>
+      <c r="F51">
+        <v>0.43169999999999997</v>
+      </c>
+      <c r="G51" t="s">
+        <v>99</v>
+      </c>
+      <c r="H51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="4">
+        <v>200000</v>
+      </c>
+      <c r="E52">
+        <v>56.05</v>
+      </c>
+      <c r="F52">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>50</v>
+      </c>
+      <c r="H52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="4">
+        <v>170000</v>
+      </c>
+      <c r="E53">
+        <v>58.02</v>
+      </c>
+      <c r="F53">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G53" t="s">
+        <v>102</v>
+      </c>
+      <c r="H53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="4">
+        <v>130000</v>
+      </c>
+      <c r="E54">
+        <v>58.02</v>
+      </c>
+      <c r="F54">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>104</v>
+      </c>
+      <c r="H54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B55" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="4">
+        <v>1505239</v>
+      </c>
+      <c r="E55">
+        <v>57.8</v>
+      </c>
+      <c r="F55">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G55" t="s">
+        <v>106</v>
+      </c>
+      <c r="H55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="4">
+        <v>1154254</v>
+      </c>
+      <c r="E56">
+        <v>57.65</v>
+      </c>
+      <c r="F56">
+        <v>0.15049999999999999</v>
+      </c>
+      <c r="G56" t="s">
+        <v>108</v>
+      </c>
+      <c r="H56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="4">
+        <v>1051121</v>
+      </c>
+      <c r="E57">
+        <v>57.65</v>
+      </c>
+      <c r="F57">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="G57" t="s">
+        <v>110</v>
+      </c>
+      <c r="H57" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
+      <formula>1000000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>